<commit_message>
adds updated queries, cretes archive folder
</commit_message>
<xml_diff>
--- a/data-raw/qry_Knights_Recaptures_EDI.xlsx
+++ b/data-raw/qry_Knights_Recaptures_EDI.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_BEA61AB9CD0DB6A02DFBF61D45F4820070DC5349" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_BEA61AB9055531AE2B1AFD854570BF5270DC5347" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB3871AE-EE94-4F88-8BD0-E0D8FA8756E0}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Recaptures___EDI_query" sheetId="1" r:id="rId1"/>
+    <sheet name="qry_Knights_Recaptures_EDI" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Recaptures___EDI_query">Recaptures___EDI_query!$A$1:$R$333</definedName>
+    <definedName name="qry_Knights_Recaptures_EDI">qry_Knights_Recaptures_EDI!$A$1:$R$333</definedName>
   </definedNames>
-  <calcPr calcId="125725" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -530,6 +541,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -17920,7 +17934,7 @@
         <v>616</v>
       </c>
       <c r="F329" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G329" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
adds updated queries, cleans catch metadata
</commit_message>
<xml_diff>
--- a/data-raw/qry_Knights_Recaptures_EDI.xlsx
+++ b/data-raw/qry_Knights_Recaptures_EDI.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_BEA61AB9055531AE2B1AFD854570BF5270DC5347" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB3871AE-EE94-4F88-8BD0-E0D8FA8756E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_BEA61AB9057537FAAF3BE2854570BF5270DC5347" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="23895" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,21 +13,10 @@
   <definedNames>
     <definedName name="qry_Knights_Recaptures_EDI">qry_Knights_Recaptures_EDI!$A$1:$R$333</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="125725" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -541,9 +530,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="11" max="11" width="11" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">

</xml_diff>